<commit_message>
adicionar usuarios em batelada funcionando
</commit_message>
<xml_diff>
--- a/static/template_cadastro.xlsx
+++ b/static/template_cadastro.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sucesso em Vendas\Python\Boopt\src\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sucesso em Vendas\Python\Boopt\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C076159-1B19-4E5F-BFF8-B6DFC9205445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A85CE3-3B95-4953-ADB3-2BB72F8DA4E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2430" yWindow="795" windowWidth="17715" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="630" windowWidth="20700" windowHeight="14295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <t>Cargo/Função*</t>
   </si>
   <si>
-    <t>Unidade(s)*</t>
+    <t>Unidade(s)</t>
   </si>
 </sst>
 </file>
@@ -73,11 +73,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -108,7 +107,7 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Data de Nascimento*"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Email"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Cargo/Função*"/>
-    <tableColumn id="2" xr3:uid="{115A938C-066F-45BD-B540-6E4F353ED0B7}" name="Unidade(s)*" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{115A938C-066F-45BD-B540-6E4F353ED0B7}" name="Unidade(s)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -402,7 +401,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,7 +415,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">

</xml_diff>

<commit_message>
mais cargos adicionados na validação de dados
</commit_message>
<xml_diff>
--- a/static/template_cadastro.xlsx
+++ b/static/template_cadastro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sucesso em Vendas\Python\Boopt\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A85CE3-3B95-4953-ADB3-2BB72F8DA4E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249A725F-11ED-429C-9D60-3F09B21A64EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="630" windowWidth="20700" windowHeight="14295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4425" yWindow="645" windowWidth="18195" windowHeight="14295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,7 +437,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="E2" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>"Atendente,Diretor Comercial,Gerente de Loja,Regional,Supervisor de Loja,Vendedor"</formula1>
+      <formula1>"Atendente,Auxiliar,CEO,Caixa,Consultor,Diretor,Gerente,Líder,Multiplicador,RH,Regional,Regional,Subgerente,Supervisor,Televendas,Vendedor"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>